<commit_message>
Auto commit - 07291744
</commit_message>
<xml_diff>
--- a/IM/202507_Service_Count_Report.xlsx
+++ b/IM/202507_Service_Count_Report.xlsx
@@ -816,22 +816,22 @@
     <t>2025-07-04</t>
   </si>
   <si>
+    <t>12:12:00</t>
+  </si>
+  <si>
+    <t>THILF02301</t>
+  </si>
+  <si>
+    <t>新北市蘆洲區永平街30號</t>
+  </si>
+  <si>
+    <t>蘆洲樂平店</t>
+  </si>
+  <si>
     <t>12:09:00</t>
   </si>
   <si>
-    <t>THILF02301</t>
-  </si>
-  <si>
-    <t>新北市蘆洲區永平街30號</t>
-  </si>
-  <si>
-    <t>蘆洲樂平店</t>
-  </si>
-  <si>
     <t>重新啟動，設定及連線皆為正常</t>
-  </si>
-  <si>
-    <t>12:12:00</t>
   </si>
   <si>
     <t>14:16:00</t>
@@ -1235,24 +1235,24 @@
     <t>10:20:00</t>
   </si>
   <si>
+    <t>10:56:00</t>
+  </si>
+  <si>
+    <t>THILF04084</t>
+  </si>
+  <si>
+    <t>新北市三重區環河南路221巷14號及16號1樓全部</t>
+  </si>
+  <si>
+    <t>三重昌隆店</t>
+  </si>
+  <si>
     <t>10:47:00</t>
-  </si>
-  <si>
-    <t>THILF04084</t>
-  </si>
-  <si>
-    <t>新北市三重區環河南路221巷14號及16號1樓全部</t>
-  </si>
-  <si>
-    <t>三重昌隆店</t>
   </si>
   <si>
     <t>更換掃描槍
 換下8119006850
 換上8119012234</t>
-  </si>
-  <si>
-    <t>10:56:00</t>
   </si>
   <si>
     <t>11:38:00</t>
@@ -5946,7 +5946,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="7">
-        <v>2025070955</v>
+        <v>2025070954</v>
       </c>
       <c r="C39" s="7">
         <v>1</v>
@@ -5983,14 +5983,16 @@
       </c>
       <c r="N39" s="8"/>
       <c r="O39" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
         <v>25400</v>
       </c>
-      <c r="S39" s="7"/>
+      <c r="S39" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T39" s="7"/>
       <c r="U39" s="7"/>
       <c r="V39" s="7"/>
@@ -6012,7 +6014,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3">
-        <v>2025070954</v>
+        <v>2025070955</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
@@ -6049,16 +6051,14 @@
       </c>
       <c r="N40" s="6"/>
       <c r="O40" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3">
         <v>25400</v>
       </c>
-      <c r="S40" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S40" s="3"/>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
@@ -6708,7 +6708,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>2025072194</v>
+        <v>2025072193</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
@@ -6747,7 +6747,7 @@
         <v>188</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P50" s="3"/>
       <c r="Q50" s="3">
@@ -6756,7 +6756,9 @@
       <c r="R50" s="3">
         <v>42458</v>
       </c>
-      <c r="S50" s="3"/>
+      <c r="S50" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
@@ -6778,7 +6780,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="7">
-        <v>2025072193</v>
+        <v>2025072194</v>
       </c>
       <c r="C51" s="7">
         <v>1</v>
@@ -6817,7 +6819,7 @@
         <v>188</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P51" s="7"/>
       <c r="Q51" s="7">
@@ -6826,9 +6828,7 @@
       <c r="R51" s="7">
         <v>42458</v>
       </c>
-      <c r="S51" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S51" s="7"/>
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
       <c r="V51" s="7"/>
@@ -7986,7 +7986,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="7">
-        <v>2025070632</v>
+        <v>2025070719</v>
       </c>
       <c r="C69" s="7">
         <v>1</v>
@@ -8009,12 +8009,8 @@
       <c r="I69" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="J69" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="K69" s="7" t="s">
-        <v>242</v>
-      </c>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
       <c r="L69" s="8" t="s">
         <v>229</v>
       </c>
@@ -8025,22 +8021,26 @@
         <v>264</v>
       </c>
       <c r="O69" s="7" t="s">
-        <v>245</v>
+        <v>39</v>
       </c>
       <c r="P69" s="7"/>
       <c r="Q69" s="7"/>
       <c r="R69" s="7">
         <v>0</v>
       </c>
-      <c r="S69" s="7"/>
+      <c r="S69" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T69" s="7"/>
       <c r="U69" s="7"/>
       <c r="V69" s="7"/>
       <c r="W69" s="7"/>
       <c r="X69" s="7"/>
-      <c r="Y69" s="7"/>
+      <c r="Y69" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="Z69" s="8" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
       <c r="AA69" s="7" t="s">
         <v>40</v>
@@ -8054,7 +8054,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="3">
-        <v>2025070719</v>
+        <v>2025070632</v>
       </c>
       <c r="C70" s="3">
         <v>1</v>
@@ -8072,13 +8072,17 @@
         <v>177</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
+      <c r="J70" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="L70" s="6" t="s">
         <v>229</v>
       </c>
@@ -8089,26 +8093,22 @@
         <v>264</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>39</v>
+        <v>245</v>
       </c>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
       <c r="R70" s="3">
         <v>0</v>
       </c>
-      <c r="S70" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S70" s="3"/>
       <c r="T70" s="3"/>
       <c r="U70" s="3"/>
       <c r="V70" s="3"/>
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
-      <c r="Y70" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="Y70" s="3"/>
       <c r="Z70" s="6" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="AA70" s="3" t="s">
         <v>40</v>
@@ -9399,7 +9399,7 @@
         <v>225</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>73</v>
@@ -9929,7 +9929,7 @@
         <v>31</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>73</v>
@@ -10246,7 +10246,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="7">
-        <v>2025071334</v>
+        <v>2025071364</v>
       </c>
       <c r="C103" s="7">
         <v>1</v>
@@ -10269,12 +10269,8 @@
       <c r="I103" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="J103" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="K103" s="7" t="s">
-        <v>242</v>
-      </c>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
       <c r="L103" s="8" t="s">
         <v>229</v>
       </c>
@@ -10285,14 +10281,16 @@
         <v>399</v>
       </c>
       <c r="O103" s="7" t="s">
-        <v>245</v>
+        <v>39</v>
       </c>
       <c r="P103" s="7"/>
       <c r="Q103" s="7"/>
       <c r="R103" s="7">
         <v>0</v>
       </c>
-      <c r="S103" s="7"/>
+      <c r="S103" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T103" s="7"/>
       <c r="U103" s="7"/>
       <c r="V103" s="7"/>
@@ -10300,7 +10298,7 @@
       <c r="X103" s="7"/>
       <c r="Y103" s="7"/>
       <c r="Z103" s="8" t="s">
-        <v>400</v>
+        <v>232</v>
       </c>
       <c r="AA103" s="7" t="s">
         <v>40</v>
@@ -10314,7 +10312,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="3">
-        <v>2025071364</v>
+        <v>2025071334</v>
       </c>
       <c r="C104" s="3">
         <v>1</v>
@@ -10332,13 +10330,17 @@
         <v>395</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I104" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="J104" s="3"/>
-      <c r="K104" s="3"/>
+      <c r="J104" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="L104" s="6" t="s">
         <v>229</v>
       </c>
@@ -10349,16 +10351,14 @@
         <v>399</v>
       </c>
       <c r="O104" s="3" t="s">
-        <v>39</v>
+        <v>245</v>
       </c>
       <c r="P104" s="3"/>
       <c r="Q104" s="3"/>
       <c r="R104" s="3">
         <v>0</v>
       </c>
-      <c r="S104" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S104" s="3"/>
       <c r="T104" s="3"/>
       <c r="U104" s="3"/>
       <c r="V104" s="3"/>
@@ -10366,7 +10366,7 @@
       <c r="X104" s="3"/>
       <c r="Y104" s="3"/>
       <c r="Z104" s="6" t="s">
-        <v>232</v>
+        <v>401</v>
       </c>
       <c r="AA104" s="3" t="s">
         <v>40</v>
@@ -14000,7 +14000,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="7">
-        <v>2025071355</v>
+        <v>2025071354</v>
       </c>
       <c r="C159" s="7">
         <v>1</v>
@@ -14039,7 +14039,7 @@
         <v>571</v>
       </c>
       <c r="O159" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P159" s="7"/>
       <c r="Q159" s="7">
@@ -14048,7 +14048,9 @@
       <c r="R159" s="7">
         <v>135890</v>
       </c>
-      <c r="S159" s="7"/>
+      <c r="S159" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T159" s="7"/>
       <c r="U159" s="7"/>
       <c r="V159" s="7"/>
@@ -14070,7 +14072,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="3">
-        <v>2025071354</v>
+        <v>2025071355</v>
       </c>
       <c r="C160" s="3">
         <v>1</v>
@@ -14109,7 +14111,7 @@
         <v>571</v>
       </c>
       <c r="O160" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P160" s="3"/>
       <c r="Q160" s="3">
@@ -14118,9 +14120,7 @@
       <c r="R160" s="3">
         <v>135890</v>
       </c>
-      <c r="S160" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S160" s="3"/>
       <c r="T160" s="3"/>
       <c r="U160" s="3"/>
       <c r="V160" s="3"/>
@@ -16432,7 +16432,7 @@
         <v>192</v>
       </c>
       <c r="B194" s="3">
-        <v>2025070748</v>
+        <v>2025070747</v>
       </c>
       <c r="C194" s="3">
         <v>1</v>
@@ -16471,14 +16471,16 @@
         <v>636</v>
       </c>
       <c r="O194" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P194" s="3"/>
       <c r="Q194" s="3"/>
       <c r="R194" s="3">
         <v>163873</v>
       </c>
-      <c r="S194" s="3"/>
+      <c r="S194" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T194" s="3"/>
       <c r="U194" s="3"/>
       <c r="V194" s="3"/>
@@ -16500,7 +16502,7 @@
         <v>193</v>
       </c>
       <c r="B195" s="7">
-        <v>2025070747</v>
+        <v>2025070748</v>
       </c>
       <c r="C195" s="7">
         <v>1</v>
@@ -16539,16 +16541,14 @@
         <v>636</v>
       </c>
       <c r="O195" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P195" s="7"/>
       <c r="Q195" s="7"/>
       <c r="R195" s="7">
         <v>163873</v>
       </c>
-      <c r="S195" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S195" s="7"/>
       <c r="T195" s="7"/>
       <c r="U195" s="7"/>
       <c r="V195" s="7"/>
@@ -16700,7 +16700,7 @@
         <v>196</v>
       </c>
       <c r="B198" s="3">
-        <v>2025073292</v>
+        <v>2025073293</v>
       </c>
       <c r="C198" s="3">
         <v>1</v>
@@ -16737,16 +16737,14 @@
       </c>
       <c r="N198" s="6"/>
       <c r="O198" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P198" s="3"/>
       <c r="Q198" s="3"/>
       <c r="R198" s="3">
         <v>96600</v>
       </c>
-      <c r="S198" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S198" s="3"/>
       <c r="T198" s="3"/>
       <c r="U198" s="3"/>
       <c r="V198" s="3"/>
@@ -16768,7 +16766,7 @@
         <v>197</v>
       </c>
       <c r="B199" s="7">
-        <v>2025073293</v>
+        <v>2025073292</v>
       </c>
       <c r="C199" s="7">
         <v>1</v>
@@ -16805,14 +16803,16 @@
       </c>
       <c r="N199" s="8"/>
       <c r="O199" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P199" s="7"/>
       <c r="Q199" s="7"/>
       <c r="R199" s="7">
         <v>96600</v>
       </c>
-      <c r="S199" s="7"/>
+      <c r="S199" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T199" s="7"/>
       <c r="U199" s="7"/>
       <c r="V199" s="7"/>
@@ -17366,7 +17366,7 @@
         <v>206</v>
       </c>
       <c r="B208" s="3">
-        <v>2025072181</v>
+        <v>2025072180</v>
       </c>
       <c r="C208" s="3">
         <v>1</v>
@@ -17405,14 +17405,16 @@
         <v>665</v>
       </c>
       <c r="O208" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P208" s="3"/>
       <c r="Q208" s="3"/>
       <c r="R208" s="3">
         <v>93598</v>
       </c>
-      <c r="S208" s="3"/>
+      <c r="S208" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T208" s="3"/>
       <c r="U208" s="3"/>
       <c r="V208" s="3"/>
@@ -17422,19 +17424,15 @@
       <c r="Z208" s="6" t="s">
         <v>666</v>
       </c>
-      <c r="AA208" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB208" s="3">
-        <v>1</v>
-      </c>
+      <c r="AA208" s="3"/>
+      <c r="AB208" s="3"/>
     </row>
     <row r="209" spans="1:28">
       <c r="A209" s="7">
         <v>207</v>
       </c>
       <c r="B209" s="7">
-        <v>2025072180</v>
+        <v>2025072181</v>
       </c>
       <c r="C209" s="7">
         <v>1</v>
@@ -17473,16 +17471,14 @@
         <v>665</v>
       </c>
       <c r="O209" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P209" s="7"/>
       <c r="Q209" s="7"/>
       <c r="R209" s="7">
         <v>93598</v>
       </c>
-      <c r="S209" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S209" s="7"/>
       <c r="T209" s="7"/>
       <c r="U209" s="7"/>
       <c r="V209" s="7"/>
@@ -17492,7 +17488,9 @@
       <c r="Z209" s="8" t="s">
         <v>666</v>
       </c>
-      <c r="AA209" s="7"/>
+      <c r="AA209" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AB209" s="7"/>
     </row>
     <row r="210" spans="1:28">
@@ -18044,7 +18042,7 @@
         <v>216</v>
       </c>
       <c r="B218" s="3">
-        <v>2025070400</v>
+        <v>2025070401</v>
       </c>
       <c r="C218" s="3">
         <v>1</v>
@@ -18083,16 +18081,14 @@
         <v>682</v>
       </c>
       <c r="O218" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P218" s="3"/>
       <c r="Q218" s="3"/>
       <c r="R218" s="3">
         <v>124717</v>
       </c>
-      <c r="S218" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S218" s="3"/>
       <c r="T218" s="3"/>
       <c r="U218" s="3"/>
       <c r="V218" s="3"/>
@@ -18114,7 +18110,7 @@
         <v>217</v>
       </c>
       <c r="B219" s="7">
-        <v>2025070401</v>
+        <v>2025070400</v>
       </c>
       <c r="C219" s="7">
         <v>1</v>
@@ -18153,14 +18149,16 @@
         <v>682</v>
       </c>
       <c r="O219" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P219" s="7"/>
       <c r="Q219" s="7"/>
       <c r="R219" s="7">
         <v>124717</v>
       </c>
-      <c r="S219" s="7"/>
+      <c r="S219" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T219" s="7"/>
       <c r="U219" s="7"/>
       <c r="V219" s="7"/>
@@ -20978,7 +20976,7 @@
         <v>259</v>
       </c>
       <c r="B261" s="7">
-        <v>2025070742</v>
+        <v>2025070741</v>
       </c>
       <c r="C261" s="7">
         <v>1</v>
@@ -21017,14 +21015,16 @@
         <v>579</v>
       </c>
       <c r="O261" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P261" s="7"/>
       <c r="Q261" s="7"/>
       <c r="R261" s="7">
         <v>144678</v>
       </c>
-      <c r="S261" s="7"/>
+      <c r="S261" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T261" s="7"/>
       <c r="U261" s="7"/>
       <c r="V261" s="7"/>
@@ -21046,7 +21046,7 @@
         <v>260</v>
       </c>
       <c r="B262" s="3">
-        <v>2025070741</v>
+        <v>2025070742</v>
       </c>
       <c r="C262" s="3">
         <v>1</v>
@@ -21085,16 +21085,14 @@
         <v>579</v>
       </c>
       <c r="O262" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P262" s="3"/>
       <c r="Q262" s="3"/>
       <c r="R262" s="3">
         <v>144678</v>
       </c>
-      <c r="S262" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S262" s="3"/>
       <c r="T262" s="3"/>
       <c r="U262" s="3"/>
       <c r="V262" s="3"/>
@@ -26170,7 +26168,7 @@
         <v>336</v>
       </c>
       <c r="B338" s="3">
-        <v>2025071393</v>
+        <v>2025071382</v>
       </c>
       <c r="C338" s="3">
         <v>1</v>
@@ -26236,7 +26234,7 @@
         <v>337</v>
       </c>
       <c r="B339" s="7">
-        <v>2025071382</v>
+        <v>2025071393</v>
       </c>
       <c r="C339" s="7">
         <v>1</v>
@@ -26774,7 +26772,7 @@
         <v>345</v>
       </c>
       <c r="B347" s="7">
-        <v>2025070085</v>
+        <v>2025070364</v>
       </c>
       <c r="C347" s="7">
         <v>1</v>
@@ -26797,12 +26795,8 @@
       <c r="I347" s="7" t="s">
         <v>917</v>
       </c>
-      <c r="J347" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="K347" s="7" t="s">
-        <v>242</v>
-      </c>
+      <c r="J347" s="7"/>
+      <c r="K347" s="7"/>
       <c r="L347" s="8" t="s">
         <v>229</v>
       </c>
@@ -26813,14 +26807,16 @@
         <v>919</v>
       </c>
       <c r="O347" s="7" t="s">
-        <v>245</v>
+        <v>39</v>
       </c>
       <c r="P347" s="7"/>
       <c r="Q347" s="7"/>
       <c r="R347" s="7">
         <v>0</v>
       </c>
-      <c r="S347" s="7"/>
+      <c r="S347" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T347" s="7"/>
       <c r="U347" s="7"/>
       <c r="V347" s="7"/>
@@ -26828,7 +26824,7 @@
       <c r="X347" s="7"/>
       <c r="Y347" s="7"/>
       <c r="Z347" s="8" t="s">
-        <v>922</v>
+        <v>232</v>
       </c>
       <c r="AA347" s="7" t="s">
         <v>40</v>
@@ -26840,7 +26836,7 @@
         <v>346</v>
       </c>
       <c r="B348" s="3">
-        <v>2025070364</v>
+        <v>2025070085</v>
       </c>
       <c r="C348" s="3">
         <v>1</v>
@@ -26863,8 +26859,12 @@
       <c r="I348" s="3" t="s">
         <v>917</v>
       </c>
-      <c r="J348" s="3"/>
-      <c r="K348" s="3"/>
+      <c r="J348" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="K348" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="L348" s="6" t="s">
         <v>229</v>
       </c>
@@ -26875,16 +26875,14 @@
         <v>919</v>
       </c>
       <c r="O348" s="3" t="s">
-        <v>39</v>
+        <v>245</v>
       </c>
       <c r="P348" s="3"/>
       <c r="Q348" s="3"/>
       <c r="R348" s="3">
         <v>0</v>
       </c>
-      <c r="S348" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S348" s="3"/>
       <c r="T348" s="3"/>
       <c r="U348" s="3"/>
       <c r="V348" s="3"/>
@@ -26892,7 +26890,7 @@
       <c r="X348" s="3"/>
       <c r="Y348" s="3"/>
       <c r="Z348" s="6" t="s">
-        <v>232</v>
+        <v>922</v>
       </c>
       <c r="AA348" s="3" t="s">
         <v>40</v>
@@ -27528,7 +27526,7 @@
         <v>944</v>
       </c>
       <c r="AB358" s="9">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit - 07291754
</commit_message>
<xml_diff>
--- a/IM/202507_Service_Count_Report.xlsx
+++ b/IM/202507_Service_Count_Report.xlsx
@@ -1235,7 +1235,7 @@
     <t>10:20:00</t>
   </si>
   <si>
-    <t>10:56:00</t>
+    <t>10:47:00</t>
   </si>
   <si>
     <t>THILF04084</t>
@@ -1245,9 +1245,6 @@
   </si>
   <si>
     <t>三重昌隆店</t>
-  </si>
-  <si>
-    <t>10:47:00</t>
   </si>
   <si>
     <t>更換掃描槍
@@ -1255,10 +1252,16 @@
 換上8119012234</t>
   </si>
   <si>
-    <t>11:38:00</t>
+    <t>10:56:00</t>
+  </si>
+  <si>
+    <t>11:36:00</t>
   </si>
   <si>
     <t>THILF04098</t>
+  </si>
+  <si>
+    <t>急修件</t>
   </si>
   <si>
     <t>新北市三重區仁美街96巷1號1樓全部</t>
@@ -1272,10 +1275,7 @@
 換上8155006307</t>
   </si>
   <si>
-    <t>11:36:00</t>
-  </si>
-  <si>
-    <t>急修件</t>
+    <t>11:38:00</t>
   </si>
   <si>
     <t>15:13:00</t>
@@ -3626,7 +3626,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>2025072178</v>
+        <v>2025072179</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -3665,7 +3665,7 @@
         <v>30</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7">
@@ -3674,9 +3674,7 @@
       <c r="R5" s="7">
         <v>3376</v>
       </c>
-      <c r="S5" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
@@ -3698,7 +3696,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>2025072179</v>
+        <v>2025072178</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -3737,7 +3735,7 @@
         <v>30</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3">
@@ -3746,7 +3744,9 @@
       <c r="R6" s="3">
         <v>3376</v>
       </c>
-      <c r="S6" s="3"/>
+      <c r="S6" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
@@ -4948,7 +4948,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3">
-        <v>2025072638</v>
+        <v>2025072639</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -4985,36 +4985,36 @@
       </c>
       <c r="N24" s="6"/>
       <c r="O24" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3">
         <v>28565</v>
       </c>
-      <c r="S24" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S24" s="3"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
-      <c r="Y24" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="Y24" s="3"/>
       <c r="Z24" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="AA24" s="3"/>
-      <c r="AB24" s="3"/>
+      <c r="AA24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:28">
       <c r="A25" s="7">
         <v>23</v>
       </c>
       <c r="B25" s="7">
-        <v>2025072639</v>
+        <v>2025072638</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
@@ -5051,26 +5051,28 @@
       </c>
       <c r="N25" s="8"/>
       <c r="O25" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="7">
         <v>28565</v>
       </c>
-      <c r="S25" s="7"/>
+      <c r="S25" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="7"/>
-      <c r="Y25" s="7"/>
+      <c r="Y25" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="Z25" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AA25" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA25" s="7"/>
       <c r="AB25" s="7"/>
     </row>
     <row r="26" spans="1:28">
@@ -7322,7 +7324,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="7">
-        <v>2025073230</v>
+        <v>2025073231</v>
       </c>
       <c r="C59" s="7">
         <v>1</v>
@@ -7361,16 +7363,14 @@
         <v>220</v>
       </c>
       <c r="O59" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P59" s="7"/>
       <c r="Q59" s="7"/>
       <c r="R59" s="7">
         <v>122223</v>
       </c>
-      <c r="S59" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S59" s="7"/>
       <c r="T59" s="7"/>
       <c r="U59" s="7"/>
       <c r="V59" s="7"/>
@@ -7380,15 +7380,19 @@
       <c r="Z59" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AA59" s="7"/>
-      <c r="AB59" s="7"/>
+      <c r="AA59" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB59" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:28">
       <c r="A60" s="3">
         <v>58</v>
       </c>
       <c r="B60" s="3">
-        <v>2025073231</v>
+        <v>2025073230</v>
       </c>
       <c r="C60" s="3">
         <v>1</v>
@@ -7427,14 +7431,16 @@
         <v>220</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
       <c r="R60" s="3">
         <v>122223</v>
       </c>
-      <c r="S60" s="3"/>
+      <c r="S60" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
       <c r="V60" s="3"/>
@@ -7444,9 +7450,7 @@
       <c r="Z60" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AA60" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA60" s="3"/>
       <c r="AB60" s="3"/>
     </row>
     <row r="61" spans="1:28">
@@ -10246,7 +10250,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="7">
-        <v>2025071364</v>
+        <v>2025071334</v>
       </c>
       <c r="C103" s="7">
         <v>1</v>
@@ -10269,8 +10273,12 @@
       <c r="I103" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="J103" s="7"/>
-      <c r="K103" s="7"/>
+      <c r="J103" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="K103" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="L103" s="8" t="s">
         <v>229</v>
       </c>
@@ -10281,16 +10289,14 @@
         <v>399</v>
       </c>
       <c r="O103" s="7" t="s">
-        <v>39</v>
+        <v>245</v>
       </c>
       <c r="P103" s="7"/>
       <c r="Q103" s="7"/>
       <c r="R103" s="7">
         <v>0</v>
       </c>
-      <c r="S103" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S103" s="7"/>
       <c r="T103" s="7"/>
       <c r="U103" s="7"/>
       <c r="V103" s="7"/>
@@ -10298,7 +10304,7 @@
       <c r="X103" s="7"/>
       <c r="Y103" s="7"/>
       <c r="Z103" s="8" t="s">
-        <v>232</v>
+        <v>400</v>
       </c>
       <c r="AA103" s="7" t="s">
         <v>40</v>
@@ -10312,7 +10318,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="3">
-        <v>2025071334</v>
+        <v>2025071364</v>
       </c>
       <c r="C104" s="3">
         <v>1</v>
@@ -10330,17 +10336,13 @@
         <v>395</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="I104" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="J104" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="K104" s="3" t="s">
-        <v>242</v>
-      </c>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
       <c r="L104" s="6" t="s">
         <v>229</v>
       </c>
@@ -10351,14 +10353,16 @@
         <v>399</v>
       </c>
       <c r="O104" s="3" t="s">
-        <v>245</v>
+        <v>39</v>
       </c>
       <c r="P104" s="3"/>
       <c r="Q104" s="3"/>
       <c r="R104" s="3">
         <v>0</v>
       </c>
-      <c r="S104" s="3"/>
+      <c r="S104" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T104" s="3"/>
       <c r="U104" s="3"/>
       <c r="V104" s="3"/>
@@ -10366,7 +10370,7 @@
       <c r="X104" s="3"/>
       <c r="Y104" s="3"/>
       <c r="Z104" s="6" t="s">
-        <v>401</v>
+        <v>232</v>
       </c>
       <c r="AA104" s="3" t="s">
         <v>40</v>
@@ -10378,7 +10382,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="7">
-        <v>2025072312</v>
+        <v>2025072317</v>
       </c>
       <c r="C105" s="7">
         <v>1</v>
@@ -10402,7 +10406,7 @@
         <v>403</v>
       </c>
       <c r="J105" s="7" t="s">
-        <v>241</v>
+        <v>404</v>
       </c>
       <c r="K105" s="7" t="s">
         <v>242</v>
@@ -10411,10 +10415,10 @@
         <v>229</v>
       </c>
       <c r="M105" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N105" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="O105" s="7" t="s">
         <v>245</v>
@@ -10432,7 +10436,7 @@
       <c r="X105" s="7"/>
       <c r="Y105" s="7"/>
       <c r="Z105" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AA105" s="7" t="s">
         <v>40</v>
@@ -10446,7 +10450,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="3">
-        <v>2025072317</v>
+        <v>2025072312</v>
       </c>
       <c r="C106" s="3">
         <v>1</v>
@@ -10464,13 +10468,13 @@
         <v>44</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="I106" s="3" t="s">
         <v>403</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>408</v>
+        <v>241</v>
       </c>
       <c r="K106" s="3" t="s">
         <v>242</v>
@@ -10479,10 +10483,10 @@
         <v>229</v>
       </c>
       <c r="M106" s="6" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N106" s="6" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="O106" s="3" t="s">
         <v>245</v>
@@ -10500,7 +10504,7 @@
       <c r="X106" s="3"/>
       <c r="Y106" s="3"/>
       <c r="Z106" s="6" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AA106" s="3" t="s">
         <v>40</v>
@@ -10541,10 +10545,10 @@
         <v>229</v>
       </c>
       <c r="M107" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N107" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="O107" s="7" t="s">
         <v>39</v>
@@ -10996,7 +11000,7 @@
         <v>177</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I114" s="3" t="s">
         <v>429</v>
@@ -16700,7 +16704,7 @@
         <v>196</v>
       </c>
       <c r="B198" s="3">
-        <v>2025073293</v>
+        <v>2025073292</v>
       </c>
       <c r="C198" s="3">
         <v>1</v>
@@ -16737,14 +16741,16 @@
       </c>
       <c r="N198" s="6"/>
       <c r="O198" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P198" s="3"/>
       <c r="Q198" s="3"/>
       <c r="R198" s="3">
         <v>96600</v>
       </c>
-      <c r="S198" s="3"/>
+      <c r="S198" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T198" s="3"/>
       <c r="U198" s="3"/>
       <c r="V198" s="3"/>
@@ -16766,7 +16772,7 @@
         <v>197</v>
       </c>
       <c r="B199" s="7">
-        <v>2025073292</v>
+        <v>2025073293</v>
       </c>
       <c r="C199" s="7">
         <v>1</v>
@@ -16803,16 +16809,14 @@
       </c>
       <c r="N199" s="8"/>
       <c r="O199" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P199" s="7"/>
       <c r="Q199" s="7"/>
       <c r="R199" s="7">
         <v>96600</v>
       </c>
-      <c r="S199" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S199" s="7"/>
       <c r="T199" s="7"/>
       <c r="U199" s="7"/>
       <c r="V199" s="7"/>
@@ -18042,7 +18046,7 @@
         <v>216</v>
       </c>
       <c r="B218" s="3">
-        <v>2025070401</v>
+        <v>2025070400</v>
       </c>
       <c r="C218" s="3">
         <v>1</v>
@@ -18081,14 +18085,16 @@
         <v>682</v>
       </c>
       <c r="O218" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P218" s="3"/>
       <c r="Q218" s="3"/>
       <c r="R218" s="3">
         <v>124717</v>
       </c>
-      <c r="S218" s="3"/>
+      <c r="S218" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T218" s="3"/>
       <c r="U218" s="3"/>
       <c r="V218" s="3"/>
@@ -18110,7 +18116,7 @@
         <v>217</v>
       </c>
       <c r="B219" s="7">
-        <v>2025070400</v>
+        <v>2025070401</v>
       </c>
       <c r="C219" s="7">
         <v>1</v>
@@ -18149,16 +18155,14 @@
         <v>682</v>
       </c>
       <c r="O219" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P219" s="7"/>
       <c r="Q219" s="7"/>
       <c r="R219" s="7">
         <v>124717</v>
       </c>
-      <c r="S219" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S219" s="7"/>
       <c r="T219" s="7"/>
       <c r="U219" s="7"/>
       <c r="V219" s="7"/>
@@ -18448,7 +18452,7 @@
         <v>222</v>
       </c>
       <c r="B224" s="3">
-        <v>2025073112</v>
+        <v>2025073113</v>
       </c>
       <c r="C224" s="3">
         <v>1</v>
@@ -18487,16 +18491,14 @@
         <v>690</v>
       </c>
       <c r="O224" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P224" s="3"/>
       <c r="Q224" s="3"/>
       <c r="R224" s="3">
         <v>33929</v>
       </c>
-      <c r="S224" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S224" s="3"/>
       <c r="T224" s="3"/>
       <c r="U224" s="3"/>
       <c r="V224" s="3"/>
@@ -18506,15 +18508,19 @@
       <c r="Z224" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="AA224" s="3"/>
-      <c r="AB224" s="3"/>
+      <c r="AA224" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB224" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="225" spans="1:28">
       <c r="A225" s="7">
         <v>223</v>
       </c>
       <c r="B225" s="7">
-        <v>2025073113</v>
+        <v>2025073112</v>
       </c>
       <c r="C225" s="7">
         <v>1</v>
@@ -18553,14 +18559,16 @@
         <v>690</v>
       </c>
       <c r="O225" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P225" s="7"/>
       <c r="Q225" s="7"/>
       <c r="R225" s="7">
         <v>33929</v>
       </c>
-      <c r="S225" s="7"/>
+      <c r="S225" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T225" s="7"/>
       <c r="U225" s="7"/>
       <c r="V225" s="7"/>
@@ -18570,9 +18578,7 @@
       <c r="Z225" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="AA225" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="AA225" s="7"/>
       <c r="AB225" s="7"/>
     </row>
     <row r="226" spans="1:28">
@@ -21388,7 +21394,7 @@
         <v>265</v>
       </c>
       <c r="B267" s="7">
-        <v>2025070749</v>
+        <v>2025070750</v>
       </c>
       <c r="C267" s="7">
         <v>1</v>
@@ -21427,16 +21433,14 @@
         <v>761</v>
       </c>
       <c r="O267" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P267" s="7"/>
       <c r="Q267" s="7"/>
       <c r="R267" s="7">
         <v>122901</v>
       </c>
-      <c r="S267" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S267" s="7"/>
       <c r="T267" s="7"/>
       <c r="U267" s="7"/>
       <c r="V267" s="7"/>
@@ -21458,7 +21462,7 @@
         <v>266</v>
       </c>
       <c r="B268" s="3">
-        <v>2025070750</v>
+        <v>2025070749</v>
       </c>
       <c r="C268" s="3">
         <v>1</v>
@@ -21497,14 +21501,16 @@
         <v>761</v>
       </c>
       <c r="O268" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P268" s="3"/>
       <c r="Q268" s="3"/>
       <c r="R268" s="3">
         <v>122901</v>
       </c>
-      <c r="S268" s="3"/>
+      <c r="S268" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T268" s="3"/>
       <c r="U268" s="3"/>
       <c r="V268" s="3"/>
@@ -23970,7 +23976,7 @@
         <v>303</v>
       </c>
       <c r="B305" s="7">
-        <v>2025072418</v>
+        <v>2025072417</v>
       </c>
       <c r="C305" s="7">
         <v>1</v>
@@ -24009,7 +24015,7 @@
         <v>815</v>
       </c>
       <c r="O305" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P305" s="7"/>
       <c r="Q305" s="7">
@@ -24018,7 +24024,9 @@
       <c r="R305" s="7">
         <v>154358</v>
       </c>
-      <c r="S305" s="7"/>
+      <c r="S305" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T305" s="7"/>
       <c r="U305" s="7"/>
       <c r="V305" s="7"/>
@@ -24028,19 +24036,15 @@
       <c r="Z305" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="AA305" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB305" s="7">
-        <v>1</v>
-      </c>
+      <c r="AA305" s="7"/>
+      <c r="AB305" s="7"/>
     </row>
     <row r="306" spans="1:28">
       <c r="A306" s="3">
         <v>304</v>
       </c>
       <c r="B306" s="3">
-        <v>2025072417</v>
+        <v>2025072418</v>
       </c>
       <c r="C306" s="3">
         <v>1</v>
@@ -24079,7 +24083,7 @@
         <v>815</v>
       </c>
       <c r="O306" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P306" s="3"/>
       <c r="Q306" s="3">
@@ -24088,9 +24092,7 @@
       <c r="R306" s="3">
         <v>154358</v>
       </c>
-      <c r="S306" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S306" s="3"/>
       <c r="T306" s="3"/>
       <c r="U306" s="3"/>
       <c r="V306" s="3"/>
@@ -24100,7 +24102,9 @@
       <c r="Z306" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="AA306" s="3"/>
+      <c r="AA306" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="AB306" s="3"/>
     </row>
     <row r="307" spans="1:28">
@@ -27102,7 +27106,7 @@
         <v>350</v>
       </c>
       <c r="B352" s="3">
-        <v>2025073538</v>
+        <v>2025073687</v>
       </c>
       <c r="C352" s="3">
         <v>1</v>
@@ -27125,12 +27129,8 @@
       <c r="I352" s="3" t="s">
         <v>931</v>
       </c>
-      <c r="J352" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="K352" s="3" t="s">
-        <v>242</v>
-      </c>
+      <c r="J352" s="3"/>
+      <c r="K352" s="3"/>
       <c r="L352" s="6" t="s">
         <v>229</v>
       </c>
@@ -27141,14 +27141,16 @@
         <v>933</v>
       </c>
       <c r="O352" s="3" t="s">
-        <v>245</v>
+        <v>39</v>
       </c>
       <c r="P352" s="3"/>
       <c r="Q352" s="3"/>
       <c r="R352" s="3">
         <v>0</v>
       </c>
-      <c r="S352" s="3"/>
+      <c r="S352" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="T352" s="3"/>
       <c r="U352" s="3"/>
       <c r="V352" s="3"/>
@@ -27156,7 +27158,7 @@
       <c r="X352" s="3"/>
       <c r="Y352" s="3"/>
       <c r="Z352" s="6" t="s">
-        <v>934</v>
+        <v>232</v>
       </c>
       <c r="AA352" s="3" t="s">
         <v>40</v>
@@ -27170,7 +27172,7 @@
         <v>351</v>
       </c>
       <c r="B353" s="7">
-        <v>2025073687</v>
+        <v>2025073538</v>
       </c>
       <c r="C353" s="7">
         <v>1</v>
@@ -27193,8 +27195,12 @@
       <c r="I353" s="7" t="s">
         <v>931</v>
       </c>
-      <c r="J353" s="7"/>
-      <c r="K353" s="7"/>
+      <c r="J353" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="K353" s="7" t="s">
+        <v>242</v>
+      </c>
       <c r="L353" s="8" t="s">
         <v>229</v>
       </c>
@@ -27205,16 +27211,14 @@
         <v>933</v>
       </c>
       <c r="O353" s="7" t="s">
-        <v>39</v>
+        <v>245</v>
       </c>
       <c r="P353" s="7"/>
       <c r="Q353" s="7"/>
       <c r="R353" s="7">
         <v>0</v>
       </c>
-      <c r="S353" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="S353" s="7"/>
       <c r="T353" s="7"/>
       <c r="U353" s="7"/>
       <c r="V353" s="7"/>
@@ -27222,7 +27226,7 @@
       <c r="X353" s="7"/>
       <c r="Y353" s="7"/>
       <c r="Z353" s="8" t="s">
-        <v>232</v>
+        <v>934</v>
       </c>
       <c r="AA353" s="7" t="s">
         <v>40</v>
@@ -27368,7 +27372,7 @@
         <v>354</v>
       </c>
       <c r="B356" s="3">
-        <v>2025072819</v>
+        <v>2025072799</v>
       </c>
       <c r="C356" s="3">
         <v>1</v>
@@ -27391,8 +27395,12 @@
       <c r="I356" s="3" t="s">
         <v>940</v>
       </c>
-      <c r="J356" s="3"/>
-      <c r="K356" s="3"/>
+      <c r="J356" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="K356" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="L356" s="6" t="s">
         <v>229</v>
       </c>
@@ -27403,16 +27411,14 @@
         <v>942</v>
       </c>
       <c r="O356" s="3" t="s">
-        <v>39</v>
+        <v>245</v>
       </c>
       <c r="P356" s="3"/>
       <c r="Q356" s="3"/>
       <c r="R356" s="3">
         <v>0</v>
       </c>
-      <c r="S356" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="S356" s="3"/>
       <c r="T356" s="3"/>
       <c r="U356" s="3"/>
       <c r="V356" s="3"/>
@@ -27420,7 +27426,7 @@
       <c r="X356" s="3"/>
       <c r="Y356" s="3"/>
       <c r="Z356" s="6" t="s">
-        <v>366</v>
+        <v>943</v>
       </c>
       <c r="AA356" s="3" t="s">
         <v>40</v>
@@ -27434,7 +27440,7 @@
         <v>355</v>
       </c>
       <c r="B357" s="7">
-        <v>2025072799</v>
+        <v>2025072819</v>
       </c>
       <c r="C357" s="7">
         <v>1</v>
@@ -27457,12 +27463,8 @@
       <c r="I357" s="7" t="s">
         <v>940</v>
       </c>
-      <c r="J357" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="K357" s="7" t="s">
-        <v>242</v>
-      </c>
+      <c r="J357" s="7"/>
+      <c r="K357" s="7"/>
       <c r="L357" s="8" t="s">
         <v>229</v>
       </c>
@@ -27473,14 +27475,16 @@
         <v>942</v>
       </c>
       <c r="O357" s="7" t="s">
-        <v>245</v>
+        <v>39</v>
       </c>
       <c r="P357" s="7"/>
       <c r="Q357" s="7"/>
       <c r="R357" s="7">
         <v>0</v>
       </c>
-      <c r="S357" s="7"/>
+      <c r="S357" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="T357" s="7"/>
       <c r="U357" s="7"/>
       <c r="V357" s="7"/>
@@ -27488,7 +27492,7 @@
       <c r="X357" s="7"/>
       <c r="Y357" s="7"/>
       <c r="Z357" s="8" t="s">
-        <v>943</v>
+        <v>366</v>
       </c>
       <c r="AA357" s="7" t="s">
         <v>40</v>
@@ -27526,7 +27530,7 @@
         <v>944</v>
       </c>
       <c r="AB358" s="9">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>